<commit_message>
replaced all app-designer files besides config with the latest app-designer files from the central git hub. Also, attempted to implement some of the user permissions, particularly for registration and delivery, but it is not working. This is an unstable commit.
</commit_message>
<xml_diff>
--- a/app/config/tables/registration/forms/registration/registration.xlsx
+++ b/app/config/tables/registration/forms/registration/registration.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/odk_repos/app-designer/app/config/tables/registration/forms/registration/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,6 +22,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>type</t>
   </si>
@@ -314,9 +322,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>MODIFY</t>
-  </si>
-  <si>
     <t>sectors</t>
   </si>
   <si>
@@ -330,6 +335,18 @@
   </si>
   <si>
     <t>What sector are you located in?</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -550,7 +567,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -587,6 +604,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -617,6 +635,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -948,7 +971,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="5" customWidth="1"/>
@@ -958,7 +981,7 @@
     <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1004,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -992,7 +1015,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>25</v>
       </c>
@@ -1006,7 +1029,7 @@
       </c>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
@@ -1020,7 +1043,7 @@
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1037,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1065,7 +1088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
@@ -1073,16 +1096,16 @@
         <v>90</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -1096,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1130,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -1124,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1158,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1149,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -1163,7 +1186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1205,7 +1228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1222,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>80</v>
       </c>
@@ -1233,7 +1256,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -1244,11 +1267,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1260,7 +1278,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" style="7" customWidth="1"/>
@@ -1268,7 +1286,7 @@
     <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1295,7 +1313,7 @@
         <v>20160805</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1303,7 +1321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1311,7 +1329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1321,11 +1339,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1337,14 +1350,14 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="26" style="5"/>
     <col min="3" max="16384" width="26" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +1373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1368,7 +1381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1384,7 +1397,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1400,7 +1413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1421,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1416,7 +1429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1424,7 +1437,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1445,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1456,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1472,7 +1485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1501,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1509,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1504,7 +1517,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>80</v>
       </c>
@@ -1515,11 +1528,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1531,7 +1539,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="17" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="17"/>
@@ -1539,7 +1547,7 @@
     <col min="5" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
@@ -1553,12 +1561,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>33</v>
       </c>
@@ -1569,11 +1577,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1585,9 +1588,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
+    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>49</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1631,7 +1634,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1664,46 +1667,41 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
         <v>93</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
         <v>94</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1715,13 +1713,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" customWidth="1"/>
     <col min="2" max="2" width="81.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>75</v>
       </c>
@@ -1729,7 +1727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="225">
+    <row r="2" spans="1:2" ht="240" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1739,25 +1737,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>84</v>
       </c>
@@ -1774,7 +1767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>87</v>
       </c>
@@ -1788,15 +1781,30 @@
         <v>2</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>91</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented user permissions for demo. Scanning a barcode as superuser does not work, so I disabled the button
</commit_message>
<xml_diff>
--- a/app/config/tables/registration/forms/registration/registration.xlsx
+++ b/app/config/tables/registration/forms/registration/registration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/odk_repos/app-designer/app/config/tables/registration/forms/registration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/tables/registration/forms/registration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -340,20 +340,20 @@
     <t>HIDDEN</t>
   </si>
   <si>
-    <t>locked</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
-    <t>true</t>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -409,6 +409,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="12">
@@ -567,7 +572,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -605,6 +610,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1745,7 +1751,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1791,11 +1797,11 @@
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
         <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>98</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>99</v>

</xml_diff>